<commit_message>
Udated documentation for FHIR IG 1.0.1..again
</commit_message>
<xml_diff>
--- a/input/images/pdf/doc_version_overview.xlsx
+++ b/input/images/pdf/doc_version_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/GitBox/docUpdate/dk-medcom/input/images/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E0D646-C49B-D14B-8C02-ECC22E098658}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13AF055-446A-4F4A-8554-BFB2A6714DE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="7140" windowWidth="40340" windowHeight="18280" activeTab="2" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
+    <workbookView xWindow="7460" yWindow="10200" windowWidth="40340" windowHeight="18280" activeTab="2" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
   <si>
     <t>Github name</t>
   </si>
@@ -933,10 +933,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C130F3EC-E328-5140-93D6-E7AF92708691}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1084,6 +1084,11 @@
         <v>29</v>
       </c>
     </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1093,10 +1098,11 @@
     <hyperlink ref="E2" r:id="rId4" xr:uid="{A54A95CE-0021-8146-AB08-695FF4365883}"/>
     <hyperlink ref="E5" r:id="rId5" xr:uid="{E9F0395E-FECF-764D-A285-58A28F4A9094}"/>
     <hyperlink ref="E3" r:id="rId6" xr:uid="{4C3FD705-D7DF-EC45-9E1F-3844EF795847}"/>
+    <hyperlink ref="B18" r:id="rId7" display="https://github.com/hl7dk/dk-medcom/blob/docUpdate/input/images/carecommunication/pdf/USE%20CASES_FHIR%20Care%20Communication.pdf" xr:uid="{9384D251-8733-3544-9001-DD9030BAC79C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated with new use case for CareCommunication release
</commit_message>
<xml_diff>
--- a/input/images/pdf/doc_version_overview.xlsx
+++ b/input/images/pdf/doc_version_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/GitBox/docUpdate/dk-medcom/input/images/pdf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13AF055-446A-4F4A-8554-BFB2A6714DE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2870B9-2FEB-F943-BF8B-BCCC0FCFC317}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="10200" windowWidth="40340" windowHeight="18280" activeTab="2" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
+    <workbookView xWindow="3220" yWindow="14960" windowWidth="40340" windowHeight="18580" activeTab="2" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="3" r:id="rId1"/>
@@ -168,18 +168,6 @@
     <t>Use Cases_FHIR Korrespondancemeddelelse.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve"> t:/Igangværende opgaver/Udvidet Korrespondancemeddelelse/Use Cases/Use Cases_FHIR Care Communication_v1.1.docx</t>
-  </si>
-  <si>
-    <t>Use Cases_FHIR Care Communication_v1.1.docx</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Use Cases_FHIR Korrespondancemeddelelse_v1.1.docx</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> t:/Igangværende opgaver/Udvidet Korrespondancemeddelelse/Use Cases/Use Cases_FHIR Korrespondancemeddelelse_v1.1.docx</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -208,6 +196,18 @@
   </si>
   <si>
     <t>t:/Igangværende opgaver/Udvidet Korrespondancemeddelelse/Release version 1.0/FHIR_Korrespondancemeddelelse_v1.0.docx</t>
+  </si>
+  <si>
+    <t>Use Cases_FHIR Care Communication_v1.0.2.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Use Cases_FHIR Korrespondancemeddelelse_v1.0.2.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> t:/Igangværende opgaver/Udvidet Korrespondancemeddelelse/Use Cases/Use Cases_FHIR Korrespondancemeddelelse_v1.0.2.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> t:/Igangværende opgaver/Udvidet Korrespondancemeddelelse/Use Cases/Use Cases_FHIR Care Communication_v1.0.2.docx</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79F97E6-EACE-4143-93BD-6BDF6CD549D5}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="99" workbookViewId="0">
+    <sheetView zoomScale="99" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -936,7 +936,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,7 +944,7 @@
     <col min="1" max="1" width="54.5" customWidth="1"/>
     <col min="2" max="2" width="43.83203125" customWidth="1"/>
     <col min="3" max="3" width="46.33203125" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
+    <col min="4" max="4" width="116.33203125" customWidth="1"/>
     <col min="5" max="5" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -965,10 +965,10 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -976,16 +976,16 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1">
         <v>44225</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -993,16 +993,16 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1">
         <v>44225</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1010,16 +1010,16 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1">
         <v>44258</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1027,16 +1027,16 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1">
         <v>44258</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>

</xml_diff>